<commit_message>
products' images value was updated
</commit_message>
<xml_diff>
--- a/uploads/Пакети.xlsx
+++ b/uploads/Пакети.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Банан" sheetId="1" r:id="rId1"/>
@@ -109,15 +109,18 @@
     <t>до 2 кг</t>
   </si>
   <si>
+    <t>Білий</t>
+  </si>
+  <si>
+    <t>Шовкотрафарет</t>
+  </si>
+  <si>
+    <t>ПВД - м'який, глянець</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Шовкотрафарет</t>
-  </si>
-  <si>
-    <t>ПВД - м'який, глянець</t>
-  </si>
-  <si>
     <t>51мкм</t>
   </si>
   <si>
@@ -130,12 +133,24 @@
     <t>Пакетики банан розміром 20х30см чорного кольору ідеально підходять для пакування маленьких сувенірів, парфумерії, медикаментів для аптек.</t>
   </si>
   <si>
+    <t>Чорний</t>
+  </si>
+  <si>
+    <t>https://paketov.net.ua/wa-data/public/shop/products/78/00/78/images/2163/2163.745.jpg</t>
+  </si>
+  <si>
     <t>Пакети 20х30 типу "банан", щільністю 51мкм, рожевого кольору</t>
   </si>
   <si>
     <t>Пакетики банан розміром 20х30см рожевого кольору ідеально підходять для пакування маленьких сувенірів, парфумерії, медикаментів для аптек.</t>
   </si>
   <si>
+    <t>Рожевий</t>
+  </si>
+  <si>
+    <t>https://paketov.net.ua/wa-data/public/shop/products/26/06/626/images/2114/2114.745.jpg</t>
+  </si>
+  <si>
     <t>Пакети "Майка" 25х40см, прозорі із ручками, 51мкм, з вашим логотипом</t>
   </si>
   <si>
@@ -148,34 +163,19 @@
     <t>до 6 кг</t>
   </si>
   <si>
+    <t>Прозорий</t>
+  </si>
+  <si>
     <t>ПНД - шарудливий, матовий</t>
   </si>
   <si>
     <t>25х40см</t>
   </si>
   <si>
-    <t>Білий</t>
-  </si>
-  <si>
-    <t>Чорний</t>
-  </si>
-  <si>
-    <t>Рожевий</t>
-  </si>
-  <si>
-    <t>Прозорий</t>
-  </si>
-  <si>
-    <t>https://paketov.net.ua/wa-data/public/shop/products/06/00/6/images/2116/2116.745.jpg</t>
-  </si>
-  <si>
-    <t>https://paketov.net.ua/wa-data/public/shop/products/78/00/78/images/2163/2163.745.jpg</t>
-  </si>
-  <si>
-    <t>https://paketov.net.ua/wa-data/public/shop/products/26/06/626/images/2114/2114.745.jpg</t>
-  </si>
-  <si>
     <t>https://paketov.net.ua/wa-data/public/shop/products/94/04/494/images/2159/2159.745.jpeg</t>
+  </si>
+  <si>
+    <t>https://paketov.net.ua/wa-data/public/shop/products/06/00/6/images/2116/2116.745.jpg, https://i1.sndcdn.com/artworks-kEA9VOcE5X9zU6KA-jOjLnw-t500x500.jpg</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -663,7 +663,7 @@
         <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
         <v>30</v>
@@ -672,39 +672,39 @@
         <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="T2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="U2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="V2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="W2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -722,7 +722,7 @@
         <v>1.22</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
@@ -734,7 +734,7 @@
         <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s">
         <v>30</v>
@@ -743,39 +743,39 @@
         <v>31</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="T3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="U3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="V3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="W3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -793,7 +793,7 @@
         <v>1.22</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -805,7 +805,7 @@
         <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
         <v>30</v>
@@ -814,40 +814,40 @@
         <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Q4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="T4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="U4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="V4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="W4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:W1 A4:J4 A2:J2 L2:V2 A3:J3 L3:V3 L4:V4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:W1 A3:W4 A2:V2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -856,9 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -935,7 +933,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -953,16 +951,16 @@
         <v>3.99</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I2" t="s">
         <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="K2" t="s">
         <v>47</v>
@@ -971,43 +969,43 @@
         <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="S2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="T2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="U2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="V2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="W2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:W1 A2:J2 L2:V2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:W2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>